<commit_message>
new images + index
</commit_message>
<xml_diff>
--- a/budget/budget2023.xlsx
+++ b/budget/budget2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rakul/Desktop/SWU/lillekat.github.io/budget/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDCA784F-96D2-8447-879F-9173622DF3AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B73D2D8-6FCC-7B47-880E-3F5175D9C1D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14900" activeTab="1" xr2:uid="{D1CCE3FA-2749-BB47-B79F-67BB4C56A698}"/>
   </bookViews>
@@ -649,6 +649,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -676,7 +677,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1011,26 +1011,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="51"/>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
+      <c r="A2" s="52"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
     </row>
     <row r="3" spans="1:8" ht="28" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
@@ -1215,10 +1215,10 @@
     </row>
     <row r="10" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="52" t="s">
+      <c r="B11" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="53"/>
+      <c r="C11" s="54"/>
       <c r="D11" s="22" t="s">
         <v>17</v>
       </c>
@@ -1359,10 +1359,10 @@
     </row>
     <row r="23" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="52" t="s">
+      <c r="B24" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="53"/>
+      <c r="C24" s="54"/>
       <c r="D24" s="22" t="s">
         <v>17</v>
       </c>
@@ -1513,8 +1513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B219F9F2-A4CC-AD4F-A3F1-917E919B80E2}">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="C2" zoomScale="114" zoomScaleNormal="116" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1533,26 +1533,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="51"/>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
+      <c r="A2" s="52"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
     </row>
     <row r="3" spans="1:12" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1579,10 +1579,10 @@
       <c r="H3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="56" t="s">
+      <c r="K3" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="L3" s="57"/>
+      <c r="L3" s="58"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -1608,10 +1608,10 @@
         <f>E4*F4</f>
         <v>4500</v>
       </c>
-      <c r="K4" s="54" t="s">
+      <c r="K4" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="55"/>
+      <c r="L4" s="56"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
@@ -1798,17 +1798,17 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="K12" s="54" t="s">
+      <c r="K12" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="L12" s="55"/>
+      <c r="L12" s="56"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B13" s="52" t="s">
+      <c r="B13" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="53"/>
-      <c r="D13" s="58"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="59"/>
       <c r="K13" s="44" t="s">
         <v>33</v>
       </c>
@@ -1834,7 +1834,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="59" t="s">
+      <c r="A15" s="50" t="s">
         <v>40</v>
       </c>
       <c r="B15" s="23">
@@ -1855,7 +1855,7 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="59" t="s">
+      <c r="A16" s="50" t="s">
         <v>41</v>
       </c>
       <c r="B16" s="23">
@@ -1871,10 +1871,12 @@
       <c r="K16" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="L16" s="45"/>
+      <c r="L16" s="45">
+        <v>4002</v>
+      </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="59" t="s">
+      <c r="A17" s="50" t="s">
         <v>42</v>
       </c>
       <c r="B17" s="23">
@@ -1893,7 +1895,7 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="59" t="s">
+      <c r="A18" s="50" t="s">
         <v>43</v>
       </c>
       <c r="B18" s="23">
@@ -1912,7 +1914,7 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="59" t="s">
+      <c r="A19" s="50" t="s">
         <v>44</v>
       </c>
       <c r="B19" s="23">
@@ -1930,7 +1932,7 @@
       </c>
       <c r="L19" s="39">
         <f>SUM(L13:L18)</f>
-        <v>4225.45</v>
+        <v>8227.4500000000007</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1953,7 +1955,7 @@
       </c>
       <c r="L21" s="37">
         <f>L10-L19</f>
-        <v>10774.55</v>
+        <v>6772.5499999999993</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
attemt on fixing website
</commit_message>
<xml_diff>
--- a/budget/budget2023.xlsx
+++ b/budget/budget2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rakul/Desktop/SWU/lillekat.github.io/budget/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B73D2D8-6FCC-7B47-880E-3F5175D9C1D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDCA784F-96D2-8447-879F-9173622DF3AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14900" activeTab="1" xr2:uid="{D1CCE3FA-2749-BB47-B79F-67BB4C56A698}"/>
   </bookViews>
@@ -649,7 +649,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -677,6 +676,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1011,26 +1011,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="52"/>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
+      <c r="A2" s="51"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
     </row>
     <row r="3" spans="1:8" ht="28" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
@@ -1215,10 +1215,10 @@
     </row>
     <row r="10" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="53" t="s">
+      <c r="B11" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="54"/>
+      <c r="C11" s="53"/>
       <c r="D11" s="22" t="s">
         <v>17</v>
       </c>
@@ -1359,10 +1359,10 @@
     </row>
     <row r="23" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="53" t="s">
+      <c r="B24" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="54"/>
+      <c r="C24" s="53"/>
       <c r="D24" s="22" t="s">
         <v>17</v>
       </c>
@@ -1513,8 +1513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B219F9F2-A4CC-AD4F-A3F1-917E919B80E2}">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" zoomScale="114" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="116" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1533,26 +1533,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="52"/>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
+      <c r="A2" s="51"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
     </row>
     <row r="3" spans="1:12" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1579,10 +1579,10 @@
       <c r="H3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="57" t="s">
+      <c r="K3" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="L3" s="58"/>
+      <c r="L3" s="57"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -1608,10 +1608,10 @@
         <f>E4*F4</f>
         <v>4500</v>
       </c>
-      <c r="K4" s="55" t="s">
+      <c r="K4" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="56"/>
+      <c r="L4" s="55"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
@@ -1798,17 +1798,17 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="K12" s="55" t="s">
+      <c r="K12" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="L12" s="56"/>
+      <c r="L12" s="55"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B13" s="53" t="s">
+      <c r="B13" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="54"/>
-      <c r="D13" s="59"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="58"/>
       <c r="K13" s="44" t="s">
         <v>33</v>
       </c>
@@ -1834,7 +1834,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="50" t="s">
+      <c r="A15" s="59" t="s">
         <v>40</v>
       </c>
       <c r="B15" s="23">
@@ -1855,7 +1855,7 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="50" t="s">
+      <c r="A16" s="59" t="s">
         <v>41</v>
       </c>
       <c r="B16" s="23">
@@ -1871,12 +1871,10 @@
       <c r="K16" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="L16" s="45">
-        <v>4002</v>
-      </c>
+      <c r="L16" s="45"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="50" t="s">
+      <c r="A17" s="59" t="s">
         <v>42</v>
       </c>
       <c r="B17" s="23">
@@ -1895,7 +1893,7 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="50" t="s">
+      <c r="A18" s="59" t="s">
         <v>43</v>
       </c>
       <c r="B18" s="23">
@@ -1914,7 +1912,7 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="50" t="s">
+      <c r="A19" s="59" t="s">
         <v>44</v>
       </c>
       <c r="B19" s="23">
@@ -1932,7 +1930,7 @@
       </c>
       <c r="L19" s="39">
         <f>SUM(L13:L18)</f>
-        <v>8227.4500000000007</v>
+        <v>4225.45</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1955,7 +1953,7 @@
       </c>
       <c r="L21" s="37">
         <f>L10-L19</f>
-        <v>6772.5499999999993</v>
+        <v>10774.55</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
budget and image update
</commit_message>
<xml_diff>
--- a/budget/budget2023.xlsx
+++ b/budget/budget2023.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rakul/Desktop/SWU/lillekat.github.io/budget/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felicia/Desktop/lille_kat/lillekat.github.io/budget/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B8BCF1C-C3C0-764D-A0AA-64D3058BEA62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804B27A2-9506-FB4D-A38F-F32991AFBE2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14900" activeTab="1" xr2:uid="{D1CCE3FA-2749-BB47-B79F-67BB4C56A698}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" activeTab="2" xr2:uid="{D1CCE3FA-2749-BB47-B79F-67BB4C56A698}"/>
   </bookViews>
   <sheets>
     <sheet name="2022" sheetId="1" r:id="rId1"/>
     <sheet name="2023" sheetId="2" r:id="rId2"/>
+    <sheet name="2024" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="53">
   <si>
     <t>Lillekat 2022 budget</t>
   </si>
@@ -173,6 +174,27 @@
   </si>
   <si>
     <t>Nr. til bestilling</t>
+  </si>
+  <si>
+    <t>Lillekat 2024 budget</t>
+  </si>
+  <si>
+    <t>Lillekat2024-06</t>
+  </si>
+  <si>
+    <t>Lillekat2024-01</t>
+  </si>
+  <si>
+    <t>Lillekat2024-03</t>
+  </si>
+  <si>
+    <t>Lillekat2024-04</t>
+  </si>
+  <si>
+    <t>Lillekat2024-05</t>
+  </si>
+  <si>
+    <t>penge på snacks</t>
   </si>
 </sst>
 </file>
@@ -183,7 +205,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;kr.&quot;_-;\-* #,##0.00\ &quot;kr.&quot;_-;_-* &quot;-&quot;??\ &quot;kr.&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;kr.&quot;"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -246,6 +268,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -584,7 +611,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -677,6 +704,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -696,9 +724,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -736,7 +764,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -842,7 +870,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -984,7 +1012,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1513,8 +1541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B219F9F2-A4CC-AD4F-A3F1-917E919B80E2}">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView zoomScale="114" zoomScaleNormal="116" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1982,4 +2010,245 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE3C72BB-923F-DB4A-A4B9-C9C78647B110}">
+  <dimension ref="A1:K12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.1640625" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="51" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="52"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+    </row>
+    <row r="3" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="57" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" s="58"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="2">
+        <v>45331</v>
+      </c>
+      <c r="C4" s="4">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>61</v>
+      </c>
+      <c r="E4" s="60">
+        <v>1475</v>
+      </c>
+      <c r="F4" s="32"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="34"/>
+      <c r="J4" s="55" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="56"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="7">
+        <v>45345</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="34"/>
+      <c r="J5" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="48">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="7">
+        <v>45366</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="34"/>
+      <c r="J6" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="7">
+        <v>45387</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="34"/>
+      <c r="J7" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="7">
+        <v>45401</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="34"/>
+      <c r="J8" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="7">
+        <v>45415</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="34"/>
+      <c r="J9" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="K9" s="41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="20"/>
+      <c r="C10" s="35">
+        <f>SUM(C4:C9)</f>
+        <v>12</v>
+      </c>
+      <c r="D10" s="20">
+        <f>SUM(D4:D9)</f>
+        <v>61</v>
+      </c>
+      <c r="E10" s="21">
+        <f>SUM(E4:E9)</f>
+        <v>1475</v>
+      </c>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21">
+        <f>SUM(H4:H9)</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="46">
+        <f>SUM(K5:K9)</f>
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="20"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+    </row>
+    <row r="12" spans="1:11" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J4:K4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
budget update, index update, and contestscraper readme
</commit_message>
<xml_diff>
--- a/budget/budget2023.xlsx
+++ b/budget/budget2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felicia/Desktop/lille_kat/lillekat.github.io/budget/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804B27A2-9506-FB4D-A38F-F32991AFBE2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D58537-BF08-A74C-B1CE-BFAD1E44DC69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" activeTab="2" xr2:uid="{D1CCE3FA-2749-BB47-B79F-67BB4C56A698}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" activeTab="1" xr2:uid="{D1CCE3FA-2749-BB47-B79F-67BB4C56A698}"/>
   </bookViews>
   <sheets>
     <sheet name="2022" sheetId="1" r:id="rId1"/>
@@ -677,6 +677,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -704,7 +705,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1039,26 +1039,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="52"/>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
+      <c r="A2" s="53"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
     </row>
     <row r="3" spans="1:8" ht="28" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
@@ -1243,10 +1243,10 @@
     </row>
     <row r="10" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="53" t="s">
+      <c r="B11" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="54"/>
+      <c r="C11" s="55"/>
       <c r="D11" s="22" t="s">
         <v>17</v>
       </c>
@@ -1387,10 +1387,10 @@
     </row>
     <row r="23" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="53" t="s">
+      <c r="B24" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="54"/>
+      <c r="C24" s="55"/>
       <c r="D24" s="22" t="s">
         <v>17</v>
       </c>
@@ -1541,8 +1541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B219F9F2-A4CC-AD4F-A3F1-917E919B80E2}">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView zoomScale="114" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="116" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1561,26 +1561,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="52"/>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
+      <c r="A2" s="53"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
     </row>
     <row r="3" spans="1:12" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1607,10 +1607,10 @@
       <c r="H3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="57" t="s">
+      <c r="K3" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="L3" s="58"/>
+      <c r="L3" s="59"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -1636,10 +1636,10 @@
         <f>E4*F4</f>
         <v>4500</v>
       </c>
-      <c r="K4" s="55" t="s">
+      <c r="K4" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="56"/>
+      <c r="L4" s="57"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
@@ -1826,17 +1826,17 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="K12" s="55" t="s">
+      <c r="K12" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="L12" s="56"/>
+      <c r="L12" s="57"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B13" s="53" t="s">
+      <c r="B13" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="54"/>
-      <c r="D13" s="59"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="60"/>
       <c r="K13" s="44" t="s">
         <v>33</v>
       </c>
@@ -2016,8 +2016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE3C72BB-923F-DB4A-A4B9-C9C78647B110}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2026,31 +2026,33 @@
     <col min="2" max="2" width="12.1640625" customWidth="1"/>
     <col min="4" max="4" width="16.83203125" customWidth="1"/>
     <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.1640625" customWidth="1"/>
+    <col min="11" max="11" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="52"/>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-    </row>
-    <row r="3" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="53"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+    </row>
+    <row r="3" spans="1:11" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
@@ -2075,10 +2077,10 @@
       <c r="H3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="57" t="s">
+      <c r="J3" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="K3" s="58"/>
+      <c r="K3" s="59"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -2093,16 +2095,16 @@
       <c r="D4">
         <v>61</v>
       </c>
-      <c r="E4" s="60">
+      <c r="E4" s="51">
         <v>1475</v>
       </c>
       <c r="F4" s="32"/>
       <c r="G4" s="33"/>
       <c r="H4" s="34"/>
-      <c r="J4" s="55" t="s">
+      <c r="J4" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="K4" s="56"/>
+      <c r="K4" s="57"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">

</xml_diff>